<commit_message>
Added a file with all download links
</commit_message>
<xml_diff>
--- a/SDATA/Paper/FilesAndLinks.xlsx
+++ b/SDATA/Paper/FilesAndLinks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgProjekte\Python\EIPH_WSI\SDATA\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD2D443-D929-43D5-9318-4F92EEB492E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958AEB81-67CE-4C5C-BDCA-780BC795BBCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Human" sheetId="1" r:id="rId1"/>
@@ -869,7 +869,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1047,18 +1047,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1229,23 +1217,22 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1604,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,7 +1603,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B1" t="s">
@@ -1625,10 +1612,10 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>199</v>
       </c>
       <c r="B2" t="s">
@@ -1637,10 +1624,10 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B3" t="s">
@@ -1649,10 +1636,10 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B4" t="s">
@@ -1661,10 +1648,10 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>200</v>
       </c>
       <c r="B5" t="s">
@@ -1673,10 +1660,10 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B6" t="s">
@@ -1685,10 +1672,10 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B7" t="s">
@@ -1697,22 +1684,22 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B9" t="s">
@@ -1721,10 +1708,10 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B10" t="s">
@@ -1733,10 +1720,10 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B11" t="s">
@@ -1745,10 +1732,10 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>209</v>
       </c>
       <c r="B12" t="s">
@@ -1757,7 +1744,7 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1784,7 +1771,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,7 +1781,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B1" t="s">
@@ -1803,10 +1790,10 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B2" t="s">
@@ -1815,10 +1802,10 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B3" t="s">
@@ -1827,10 +1814,10 @@
       <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B4" t="s">
@@ -1839,10 +1826,10 @@
       <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B5" t="s">
@@ -1851,10 +1838,10 @@
       <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B6" t="s">
@@ -1863,10 +1850,10 @@
       <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>215</v>
       </c>
       <c r="B7" t="s">
@@ -1875,7 +1862,7 @@
       <c r="C7" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1895,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,18 +1894,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
@@ -1927,26 +1920,32 @@
       <c r="C2" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B4" t="s">
@@ -1955,12 +1954,15 @@
       <c r="C4" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B5" t="s">
@@ -1969,12 +1971,15 @@
       <c r="C5" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B6" t="s">
@@ -1983,29 +1988,32 @@
       <c r="C6" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B8" t="s">
@@ -2014,12 +2022,15 @@
       <c r="C8" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B9" t="s">
@@ -2028,12 +2039,15 @@
       <c r="C9" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B10" t="s">
@@ -2042,26 +2056,32 @@
       <c r="C10" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B12" t="s">
@@ -2070,12 +2090,15 @@
       <c r="C12" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B13" t="s">
@@ -2084,12 +2107,15 @@
       <c r="C13" t="s">
         <v>135</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B14" t="s">
@@ -2098,12 +2124,15 @@
       <c r="C14" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B15" t="s">
@@ -2112,12 +2141,15 @@
       <c r="C15" t="s">
         <v>139</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
@@ -2126,12 +2158,15 @@
       <c r="C16" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B17" t="s">
@@ -2140,26 +2175,32 @@
       <c r="C17" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B19" t="s">
@@ -2168,12 +2209,15 @@
       <c r="C19" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B20" t="s">
@@ -2182,9 +2226,15 @@
       <c r="C20" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B21" t="s">
@@ -2242,7 +2292,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B1" t="s">
@@ -2253,7 +2303,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B2" t="s">
@@ -2264,7 +2314,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B3" t="s">
@@ -2275,7 +2325,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B4" t="s">
@@ -2286,7 +2336,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B5" t="s">
@@ -2297,7 +2347,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B6" t="s">
@@ -2308,7 +2358,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B7" t="s">
@@ -2319,7 +2369,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B8" t="s">
@@ -2330,7 +2380,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B9" t="s">
@@ -2341,7 +2391,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B10" t="s">
@@ -2352,7 +2402,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B11" t="s">
@@ -2363,7 +2413,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B12" t="s">
@@ -2374,7 +2424,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B13" t="s">
@@ -2385,7 +2435,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B14" t="s">
@@ -2396,7 +2446,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B15" t="s">
@@ -2407,7 +2457,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B16" t="s">
@@ -2418,7 +2468,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B17" t="s">
@@ -2429,7 +2479,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B18" t="s">
@@ -2483,7 +2533,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C1" t="s">
@@ -2492,10 +2542,10 @@
       <c r="D1" t="s">
         <v>177</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C2" t="s">
@@ -2506,7 +2556,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C3" t="s">
@@ -2517,7 +2567,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C4" t="s">
@@ -2528,7 +2578,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C5" t="s">
@@ -2539,7 +2589,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C6" t="s">
@@ -2569,8 +2619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2580,7 +2630,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B1" t="s">
@@ -2591,7 +2641,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B2" t="s">
@@ -2602,7 +2652,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B3" t="s">
@@ -2613,7 +2663,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B4" t="s">
@@ -2624,7 +2674,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B5" t="s">
@@ -2635,7 +2685,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B6" t="s">
@@ -2646,7 +2696,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B7" t="s">
@@ -2657,7 +2707,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B8" t="s">
@@ -2668,7 +2718,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B9" t="s">
@@ -2679,7 +2729,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B10" t="s">

</xml_diff>